<commit_message>
MaJ suite point de synchro de mercredi
</commit_message>
<xml_diff>
--- a/Planning formation.xlsx
+++ b/Planning formation.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\formation\SOPRA_ACADEMY\Angular JS\formation_angular\repo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
@@ -10,9 +15,9 @@
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
     <sheet name="Participants" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
   <si>
     <t>#</t>
   </si>
@@ -280,15 +285,18 @@
   <si>
     <t>a améliorer</t>
   </si>
+  <si>
+    <t>I18N</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -554,6 +562,9 @@
     <xf numFmtId="9" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -590,8 +601,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -865,21 +882,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="7.140625" style="20" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="27"/>
@@ -890,7 +907,7 @@
     <col min="10" max="16384" width="11.42578125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="20" customFormat="1">
+    <row r="1" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
         <v>3</v>
       </c>
@@ -919,8 +936,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="34">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="35">
         <v>1</v>
       </c>
       <c r="B2" s="2">
@@ -929,33 +946,33 @@
       <c r="C2" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="39"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="35"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="36"/>
       <c r="B3" s="2">
         <f>B2+C2</f>
         <v>0.39583333333333337</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="39"/>
-    </row>
-    <row r="4" spans="1:9" ht="28.5">
-      <c r="A4" s="35"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40"/>
+    </row>
+    <row r="4" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="36"/>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B26" si="0">B3+C3</f>
+        <f t="shared" ref="B4:B27" si="0">B3+C3</f>
         <v>0.39583333333333337</v>
       </c>
       <c r="C4" s="21">
@@ -978,8 +995,8 @@
       </c>
       <c r="I4" s="23"/>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="35"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="36"/>
       <c r="B5" s="2">
         <f t="shared" si="0"/>
         <v>0.41666666666666669</v>
@@ -1004,8 +1021,8 @@
       </c>
       <c r="I5" s="23"/>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="35"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="36"/>
       <c r="B6" s="2">
         <f t="shared" si="0"/>
         <v>0.43055555555555558</v>
@@ -1013,17 +1030,17 @@
       <c r="C6" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="33"/>
-    </row>
-    <row r="7" spans="1:9" ht="57">
-      <c r="A7" s="35"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="34"/>
+    </row>
+    <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="A7" s="36"/>
       <c r="B7" s="2">
         <f t="shared" si="0"/>
         <v>0.44097222222222227</v>
@@ -1050,8 +1067,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="35"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="36"/>
       <c r="B8" s="2">
         <f t="shared" si="0"/>
         <v>0.50347222222222232</v>
@@ -1059,23 +1076,23 @@
       <c r="C8" s="21">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="33"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="35"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="34"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="36"/>
       <c r="B9" s="2">
         <f t="shared" si="0"/>
         <v>0.54513888888888895</v>
       </c>
       <c r="C9" s="21">
-        <v>5.2083333333333336E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>13</v>
@@ -1096,14 +1113,14 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="35"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="36"/>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
-        <v>0.59722222222222232</v>
+        <v>0.58680555555555558</v>
       </c>
       <c r="C10" s="21">
-        <v>4.1666666666666664E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>14</v>
@@ -1124,29 +1141,29 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="35"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="36"/>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
-        <v>0.63888888888888895</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="C11" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="35"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="36"/>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
-        <v>0.64930555555555558</v>
+        <v>0.62847222222222221</v>
       </c>
       <c r="C12" s="21">
         <v>6.25E-2</v>
@@ -1170,341 +1187,365 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="36"/>
       <c r="B13" s="2">
         <f t="shared" si="0"/>
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="C13" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="45"/>
+      <c r="F13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="46"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="37"/>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
         <v>0.71180555555555558</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C14" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D14" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="34">
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="34"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="35">
         <v>2</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="2">
         <v>0.375</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C15" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D15" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="35"/>
-      <c r="B15" s="2">
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="40"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="36"/>
+      <c r="B16" s="2">
         <f t="shared" si="0"/>
         <v>0.38541666666666669</v>
-      </c>
-      <c r="C15" s="21">
-        <v>3.125E-2</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="3">
-        <v>7</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="23"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="35"/>
-      <c r="B16" s="2">
-        <f t="shared" si="0"/>
-        <v>0.41666666666666669</v>
       </c>
       <c r="C16" s="21">
         <v>3.125E-2</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="3">
+        <v>7</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="23"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="36"/>
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C17" s="21">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E17" s="3">
         <v>8</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I17" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="35"/>
-      <c r="B17" s="2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="36"/>
+      <c r="B18" s="2">
         <f t="shared" si="0"/>
         <v>0.44791666666666669</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C18" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D18" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="33"/>
-    </row>
-    <row r="18" spans="1:9" ht="28.5">
-      <c r="A18" s="35"/>
-      <c r="B18" s="17">
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="34"/>
+    </row>
+    <row r="19" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="36"/>
+      <c r="B19" s="17">
         <f t="shared" si="0"/>
         <v>0.45833333333333337</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C19" s="25">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E19" s="3">
         <v>9</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="G19" s="26" t="s">
         <v>26</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="28.5">
-      <c r="A19" s="35"/>
-      <c r="B19" s="2">
-        <f>B18+C18</f>
-        <v>0.5</v>
-      </c>
-      <c r="C19" s="21">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="3">
-        <v>10</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="43" t="s">
-        <v>83</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="35"/>
+      <c r="I19" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="36"/>
       <c r="B20" s="2">
-        <f t="shared" si="0"/>
-        <v>0.54166666666666663</v>
+        <f>B19+C19</f>
+        <v>0.5</v>
       </c>
       <c r="C20" s="21">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="3">
+        <v>10</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="36"/>
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C21" s="21">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D21" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="33"/>
-    </row>
-    <row r="21" spans="1:9" ht="28.5">
-      <c r="A21" s="35"/>
-      <c r="B21" s="2">
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="34"/>
+    </row>
+    <row r="22" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="36"/>
+      <c r="B22" s="2">
         <f t="shared" si="0"/>
         <v>0.58333333333333326</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C22" s="21">
         <v>6.25E-2</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E22" s="3">
         <v>11</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="G21" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="I21" s="23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="28.5">
-      <c r="A22" s="35"/>
-      <c r="B22" s="2">
-        <f t="shared" si="0"/>
-        <v>0.64583333333333326</v>
-      </c>
-      <c r="C22" s="21">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="3">
-        <v>12</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="G22" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="36"/>
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.64583333333333326</v>
+      </c>
+      <c r="C23" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="3">
+        <v>12</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="23" t="s">
+      <c r="I23" s="23" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="35"/>
-      <c r="B23" s="2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="36"/>
+      <c r="B24" s="2">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C24" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D24" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="33"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="35"/>
-      <c r="B24" s="2">
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="34"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="36"/>
+      <c r="B25" s="2">
         <f t="shared" si="0"/>
         <v>0.67708333333333326</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C25" s="21">
         <v>3.125E-2</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E25" s="3">
         <v>14</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G25" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="26" t="s">
+      <c r="H25" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I24" s="23"/>
-    </row>
-    <row r="25" spans="1:9" ht="15" customHeight="1">
-      <c r="A25" s="35"/>
-      <c r="B25" s="2">
-        <f t="shared" si="0"/>
-        <v>0.70833333333333326</v>
-      </c>
-      <c r="C25" s="21">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="42"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="I25" s="23"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="36"/>
       <c r="B26" s="2">
         <f t="shared" si="0"/>
+        <v>0.70833333333333326</v>
+      </c>
+      <c r="C26" s="21">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="43"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="37"/>
+      <c r="B27" s="2">
+        <f t="shared" si="0"/>
         <v>0.71874999999999989</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C27" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D27" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D13:I13"/>
-    <mergeCell ref="A14:A26"/>
+    <mergeCell ref="D14:I14"/>
+    <mergeCell ref="A15:A27"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="D3:I3"/>
-    <mergeCell ref="D14:I14"/>
-    <mergeCell ref="D23:I23"/>
-    <mergeCell ref="D20:I20"/>
-    <mergeCell ref="D25:I25"/>
+    <mergeCell ref="D15:I15"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="D21:I21"/>
     <mergeCell ref="D26:I26"/>
+    <mergeCell ref="D27:I27"/>
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="D8:I8"/>
     <mergeCell ref="D11:I11"/>
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="A2:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1512,14 +1553,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="8"/>
@@ -1528,7 +1569,7 @@
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1545,7 +1586,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -1562,7 +1603,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -1579,7 +1620,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -1596,7 +1637,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -1613,7 +1654,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -1630,7 +1671,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>6</v>
       </c>
@@ -1647,7 +1688,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>7</v>
       </c>
@@ -1664,7 +1705,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>8</v>
       </c>
@@ -1681,7 +1722,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>9</v>
       </c>
@@ -1698,7 +1739,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>10</v>
       </c>
@@ -1715,7 +1756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>11</v>
       </c>
@@ -1732,7 +1773,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>12</v>
       </c>

</xml_diff>